<commit_message>
fix typo on girlsIdol
</commit_message>
<xml_diff>
--- a/Questions/girlIdol.xlsx
+++ b/Questions/girlIdol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3530E715-4C2B-DB42-A072-A861481E7ED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82295BC0-B386-E742-A877-D7D056B547E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D69C574B-2446-1440-BF5C-67EC254F5BC4}"/>
   </bookViews>
@@ -47,10 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>answer keyword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이오아이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -404,6 +400,10 @@
   </si>
   <si>
     <t>pNfTK39k55U</t>
+  </si>
+  <si>
+    <t>answerKeyword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBF8C64-B11C-3A4A-B95B-1A02E237DE75}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -791,502 +791,503 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>110</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>151</v>
       </c>
       <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>121</v>
       </c>
       <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>45</v>
       </c>
       <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>146</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>96</v>
       </c>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>20</v>
       </c>
       <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>90</v>
       </c>
       <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22">
         <v>103</v>
       </c>
       <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
         <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>19</v>
       </c>
       <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
         <v>41</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29">
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30">
         <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31">
         <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32">
         <v>76</v>
       </c>
       <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
         <v>45</v>
-      </c>
-      <c r="D32" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
         <v>48</v>
-      </c>
-      <c r="D34" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35">
         <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>58</v>
       </c>
       <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
         <v>67</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37">
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38">
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40">
         <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41">
         <v>23</v>
       </c>
       <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
         <v>98</v>
-      </c>
-      <c r="D41" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>